<commit_message>
modelacao inicial do carro; timesheet update
</commit_message>
<xml_diff>
--- a/timesheet_1.xlsx
+++ b/timesheet_1.xlsx
@@ -721,7 +721,7 @@
   <dimension ref="A2:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,11 +816,11 @@
       </c>
       <c r="G9" s="38">
         <f>SUM(D9:D11)*60+SUM(F9:F11)</f>
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="H9" s="39" t="str">
         <f>CONCATENATE(QUOTIENT(G9,60),"h",IF(MOD(G9,60)&lt;10,"0",""),MOD(G9,60),"m")</f>
-        <v>0h50m</v>
+        <v>1h35m</v>
       </c>
       <c r="K9" s="1"/>
     </row>
@@ -847,11 +847,11 @@
       </c>
       <c r="C11" s="35"/>
       <c r="D11" s="34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="34"/>
       <c r="F11" s="34">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G11" s="38"/>
       <c r="H11" s="36"/>
@@ -869,15 +869,15 @@
       </c>
       <c r="E12" s="34"/>
       <c r="F12" s="34">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G12" s="38">
         <f>SUM(D12:D14)*60+SUM(F12:F14)</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="H12" s="39" t="str">
         <f>CONCATENATE(QUOTIENT(G12,60),"h",IF(MOD(G12,60)&lt;10,"0",""),MOD(G12,60),"m")</f>
-        <v>0h00m</v>
+        <v>1h15m</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -891,7 +891,7 @@
       </c>
       <c r="E13" s="34"/>
       <c r="F13" s="34">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="G13" s="38"/>
       <c r="H13" s="36"/>
@@ -976,11 +976,11 @@
       </c>
       <c r="G18" s="17">
         <f>SUM(G9:G16)</f>
-        <v>50</v>
+        <v>170</v>
       </c>
       <c r="H18" s="23" t="str">
         <f>CONCATENATE(QUOTIENT(G18,60),"h",IF(MOD(G18,60)&lt;10,"0",""),MOD(G18,60),"m")</f>
-        <v>0h50m</v>
+        <v>2h50m</v>
       </c>
     </row>
     <row r="19" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
laranja e manteiga feitos!
</commit_message>
<xml_diff>
--- a/timesheet_1.xlsx
+++ b/timesheet_1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="4632"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Timesheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -96,12 +96,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
     <numFmt numFmtId="165" formatCode="dd\,\ hh:mm"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,7 +110,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -142,30 +157,22 @@
     </font>
     <font>
       <b/>
-      <sz val="9"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
+      <b/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -297,117 +304,109 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -714,300 +713,299 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="73.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="73.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="1:15" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
+    </row>
+    <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="26" t="s">
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="31" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31" t="s">
+      <c r="E7" s="14"/>
+      <c r="F7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="32"/>
+      <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:15" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="10"/>
-      <c r="D8"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="36" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="21">
         <v>0</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34">
+      <c r="E9" s="21"/>
+      <c r="F9" s="21">
         <v>20</v>
       </c>
-      <c r="G9" s="38">
+      <c r="G9" s="22">
         <f>SUM(D9:D11)*60+SUM(F9:F11)</f>
-        <v>95</v>
-      </c>
-      <c r="H9" s="35" t="str">
+        <v>155</v>
+      </c>
+      <c r="H9" s="23" t="str">
         <f>CONCATENATE(QUOTIENT(G9,60),"h",IF(MOD(G9,60)&lt;10,"0",""),MOD(G9,60),"m")</f>
-        <v>1h35m</v>
-      </c>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="36"/>
-      <c r="B10" s="11" t="s">
+        <v>2h35m</v>
+      </c>
+      <c r="K9" s="16"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="34">
+      <c r="C10" s="20"/>
+      <c r="D10" s="21">
         <v>0</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34">
+      <c r="E10" s="21"/>
+      <c r="F10" s="21">
         <v>0</v>
       </c>
-      <c r="G10" s="38"/>
-      <c r="H10" s="36"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="36"/>
-      <c r="B11" s="11" t="s">
+      <c r="G10" s="22"/>
+      <c r="H10" s="18"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="34">
+      <c r="C11" s="24"/>
+      <c r="D11" s="21">
+        <v>2</v>
+      </c>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21">
+        <v>15</v>
+      </c>
+      <c r="G11" s="22"/>
+      <c r="H11" s="18"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="21">
+        <v>0</v>
+      </c>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21">
+        <v>30</v>
+      </c>
+      <c r="G12" s="22">
+        <f>SUM(D12:D14)*60+SUM(F12:F14)</f>
+        <v>345</v>
+      </c>
+      <c r="H12" s="23" t="str">
+        <f>CONCATENATE(QUOTIENT(G12,60),"h",IF(MOD(G12,60)&lt;10,"0",""),MOD(G12,60),"m")</f>
+        <v>5h45m</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="24"/>
+      <c r="D13" s="21">
+        <v>4</v>
+      </c>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21">
+        <v>15</v>
+      </c>
+      <c r="G13" s="22"/>
+      <c r="H13" s="18"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="24"/>
+      <c r="D14" s="21">
         <v>1</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34">
-        <v>15</v>
-      </c>
-      <c r="G11" s="38"/>
-      <c r="H11" s="36"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="36"/>
-      <c r="B12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="34">
+      <c r="E14" s="21"/>
+      <c r="F14" s="21">
         <v>0</v>
       </c>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34">
-        <v>30</v>
-      </c>
-      <c r="G12" s="38">
-        <f>SUM(D12:D14)*60+SUM(F12:F14)</f>
-        <v>285</v>
-      </c>
-      <c r="H12" s="35" t="str">
-        <f>CONCATENATE(QUOTIENT(G12,60),"h",IF(MOD(G12,60)&lt;10,"0",""),MOD(G12,60),"m")</f>
-        <v>4h45m</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="36"/>
-      <c r="B13" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="34">
-        <v>4</v>
-      </c>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34">
-        <v>15</v>
-      </c>
-      <c r="G13" s="38"/>
-      <c r="H13" s="36"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="36"/>
-      <c r="B14" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="34">
+      <c r="G14" s="22"/>
+      <c r="H14" s="18"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="21">
         <v>0</v>
       </c>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34">
+      <c r="E15" s="21"/>
+      <c r="F15" s="21">
         <v>0</v>
       </c>
-      <c r="G14" s="38"/>
-      <c r="H14" s="36"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="36"/>
-      <c r="B15" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="34">
-        <v>0</v>
-      </c>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34">
-        <v>0</v>
-      </c>
-      <c r="G15" s="38">
+      <c r="G15" s="22">
         <f>SUM(D15:D16)*60+SUM(F15:F16)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="35" t="str">
+      <c r="H15" s="23" t="str">
         <f>CONCATENATE(QUOTIENT(G15,60),"h",IF(MOD(G15,60)&lt;10,"0",""),MOD(G15,60),"m")</f>
         <v>0h00m</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="36"/>
-      <c r="B16" s="11" t="s">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="34">
+      <c r="C16" s="24"/>
+      <c r="D16" s="21">
         <v>0</v>
       </c>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34">
+      <c r="E16" s="21"/>
+      <c r="F16" s="21">
         <v>0</v>
       </c>
-      <c r="G16" s="38"/>
-      <c r="H16" s="36"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="2:13" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="9"/>
-      <c r="D17"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="16" t="s">
+      <c r="G16" s="22"/>
+      <c r="H16" s="18"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+    </row>
+    <row r="17" spans="2:13" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="25"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="31">
         <f>SUM(G9:G16)</f>
-        <v>380</v>
-      </c>
-      <c r="H18" s="23" t="str">
+        <v>500</v>
+      </c>
+      <c r="H18" s="32" t="str">
         <f>CONCATENATE(QUOTIENT(G18,60),"h",IF(MOD(G18,60)&lt;10,"0",""),MOD(G18,60),"m")</f>
-        <v>6h20m</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="33" t="s">
+        <v>8h20m</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="33"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="38" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="J23" s="1"/>
-      <c r="M23" s="1"/>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D20" s="25"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="J23" s="16"/>
+      <c r="M23" s="16"/>
     </row>
   </sheetData>
   <sheetProtection password="E05B" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
@@ -1025,11 +1023,11 @@
     <mergeCell ref="G12:G14"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9 F11:F16">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9 F11:F16" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
       <formula2>60</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10 D9 D11:D16">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10 D9 D11:D16" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>